<commit_message>
Adressed Issues: 15965, 15976, 16269, 16340, 16354, 16404, 16405, 16564, 16565, 16655, 16885, 17048, 17064, 17066, 17067, 17337
</commit_message>
<xml_diff>
--- a/docs/dds-psm-cxx-ftf-votes.xlsx
+++ b/docs/dds-psm-cxx-ftf-votes.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22624"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="3300" windowWidth="21780" windowHeight="14780" tabRatio="500"/>
+    <workbookView xWindow="1020" yWindow="960" windowWidth="24560" windowHeight="18340" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Voting Now" sheetId="2" r:id="rId1"/>
-    <sheet name="All" sheetId="1" r:id="rId2"/>
+    <sheet name="batch1" sheetId="2" r:id="rId1"/>
+    <sheet name="batch2" sheetId="5" r:id="rId2"/>
+    <sheet name="All" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,42 +20,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Angelo Corsaro</author>
-  </authors>
-  <commentList>
-    <comment ref="D4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Angelo Corsaro:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Necessary changes have been applied but considering that this is a controversial matter we should give FTF members more time to digest the implications.</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="47">
   <si>
     <t>Issue #</t>
   </si>
@@ -150,13 +117,58 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Abstain</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>The tdds namespace should be merged into the dds namespace</t>
+  </si>
+  <si>
+    <t>Expected use of AnyDataReader::get and its implication on AnyDataReader's template constructor</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Getter/Setter for member arrays</t>
+  </si>
+  <si>
+    <t>The Status API, e.g. sample_rejected_status, deadline_missed_status, etc., are missing from the DataReader</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ReaderState: the class name does not reflect the intent of the class</t>
+  </si>
+  <si>
+    <t>Assignment Rule for Container Types</t>
+  </si>
+  <si>
+    <t>Update specification for final DDS-XTypes</t>
+  </si>
+  <si>
+    <t>read/take consistency for loaned and non-loaned samples</t>
+  </si>
+  <si>
+    <t>OCI</t>
+  </si>
+  <si>
+    <t>TOC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Useless ReaderQuery on DataReader read/take </t>
+  </si>
+  <si>
+    <t>N.A.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -186,19 +198,6 @@
       <color theme="2"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -288,7 +287,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="29">
+  <cellStyleXfs count="217">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -318,8 +317,196 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -340,10 +527,10 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -352,14 +539,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="29">
+  <cellStyles count="217">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
@@ -374,6 +564,100 @@
     <cellStyle name="Lien hypertexte" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="205" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="215" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
@@ -388,6 +672,100 @@
     <cellStyle name="Lien hypertexte visité" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="216" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -719,8 +1097,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3:H9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -771,12 +1149,18 @@
       <c r="D3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="3"/>
-      <c r="G3" s="10"/>
+      <c r="E3" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="H3" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="I3" s="10"/>
+      <c r="I3" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="J3" s="10" t="s">
         <v>31</v>
       </c>
@@ -794,12 +1178,18 @@
       <c r="D4" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="3"/>
-      <c r="G4" s="10"/>
+      <c r="E4" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>33</v>
+      </c>
       <c r="H4" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="I4" s="10"/>
+      <c r="I4" s="10" t="s">
+        <v>32</v>
+      </c>
       <c r="J4" s="10" t="s">
         <v>31</v>
       </c>
@@ -817,12 +1207,18 @@
       <c r="D5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="3"/>
-      <c r="G5" s="10"/>
+      <c r="E5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="H5" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="I5" s="10"/>
+      <c r="I5" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="J5" s="10" t="s">
         <v>31</v>
       </c>
@@ -840,12 +1236,18 @@
       <c r="D6" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="3"/>
-      <c r="G6" s="10"/>
+      <c r="E6" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="H6" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="I6" s="10"/>
+      <c r="I6" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="J6" s="10" t="s">
         <v>31</v>
       </c>
@@ -863,12 +1265,18 @@
       <c r="D7" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="3"/>
-      <c r="G7" s="10"/>
+      <c r="E7" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="H7" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="I7" s="10"/>
+      <c r="I7" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="J7" s="10" t="s">
         <v>31</v>
       </c>
@@ -886,12 +1294,18 @@
       <c r="D8" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="3"/>
-      <c r="G8" s="10"/>
+      <c r="E8" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="H8" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="I8" s="10"/>
+      <c r="I8" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="J8" s="10" t="s">
         <v>31</v>
       </c>
@@ -909,12 +1323,18 @@
       <c r="D9" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="3"/>
-      <c r="G9" s="10"/>
+      <c r="E9" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="H9" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="I9" s="10"/>
+      <c r="I9" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="J9" s="10" t="s">
         <v>31</v>
       </c>
@@ -934,11 +1354,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:K22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:M18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -949,7 +1369,7 @@
     <col min="7" max="11" width="10.83203125" style="11"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11">
+    <row r="2" spans="2:13">
       <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
@@ -978,38 +1398,455 @@
       <c r="K2" s="7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="2:11">
+      <c r="L2" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13">
       <c r="B3" s="10">
         <v>15965</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="12"/>
+      <c r="D3" s="14" t="s">
+        <v>14</v>
+      </c>
       <c r="E3" s="3"/>
       <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
+      <c r="H3" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="I3" s="10"/>
       <c r="J3" s="10"/>
       <c r="K3" s="10"/>
-    </row>
-    <row r="4" spans="2:11">
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+    </row>
+    <row r="4" spans="2:13">
       <c r="B4" s="10">
         <v>15976</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="12"/>
+      <c r="D4" s="14" t="s">
+        <v>14</v>
+      </c>
       <c r="E4" s="3"/>
       <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
+      <c r="H4" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="I4" s="10"/>
       <c r="J4" s="10"/>
       <c r="K4" s="10"/>
-    </row>
-    <row r="5" spans="2:11">
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+    </row>
+    <row r="5" spans="2:13">
+      <c r="B5" s="10">
+        <v>16269</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+    </row>
+    <row r="6" spans="2:13">
+      <c r="B6" s="10">
+        <v>16340</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+    </row>
+    <row r="7" spans="2:13">
+      <c r="B7" s="10">
+        <v>16354</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+    </row>
+    <row r="8" spans="2:13">
+      <c r="B8" s="10">
+        <v>16404</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+    </row>
+    <row r="9" spans="2:13" ht="30">
+      <c r="B9" s="10">
+        <v>16405</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+    </row>
+    <row r="10" spans="2:13">
+      <c r="B10" s="10">
+        <v>16564</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+    </row>
+    <row r="11" spans="2:13">
+      <c r="B11" s="10">
+        <v>16565</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+    </row>
+    <row r="12" spans="2:13" ht="30">
+      <c r="B12" s="10">
+        <v>16655</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="3"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+    </row>
+    <row r="13" spans="2:13" ht="45">
+      <c r="B13" s="10">
+        <v>16885</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="3"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+    </row>
+    <row r="14" spans="2:13" ht="60">
+      <c r="B14" s="10">
+        <v>17048</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="3"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+    </row>
+    <row r="15" spans="2:13" ht="30">
+      <c r="B15" s="10">
+        <v>17064</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="3"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+    </row>
+    <row r="16" spans="2:13" ht="30">
+      <c r="B16" s="10">
+        <v>17066</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="3"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
+    </row>
+    <row r="17" spans="2:13">
+      <c r="B17" s="10">
+        <v>17067</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" s="3"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
+    </row>
+    <row r="18" spans="2:13" ht="30">
+      <c r="B18" s="10">
+        <v>17337</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" s="3"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:M34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:M6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="10.83203125" style="11"/>
+    <col min="3" max="3" width="35.1640625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="18.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="10.83203125" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:13">
+      <c r="B2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13">
+      <c r="B3" s="10">
+        <v>15965</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+    </row>
+    <row r="4" spans="2:13">
+      <c r="B4" s="10">
+        <v>15976</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+    </row>
+    <row r="5" spans="2:13">
       <c r="B5" s="10">
         <v>16261</v>
       </c>
@@ -1023,23 +1860,31 @@
       <c r="I5" s="10"/>
       <c r="J5" s="10"/>
       <c r="K5" s="10"/>
-    </row>
-    <row r="6" spans="2:11">
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+    </row>
+    <row r="6" spans="2:13">
       <c r="B6" s="10">
         <v>16269</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="12"/>
+      <c r="D6" s="8" t="s">
+        <v>14</v>
+      </c>
       <c r="E6" s="3"/>
       <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
+      <c r="H6" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="I6" s="10"/>
       <c r="J6" s="10"/>
       <c r="K6" s="10"/>
-    </row>
-    <row r="7" spans="2:11">
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+    </row>
+    <row r="7" spans="2:13">
       <c r="B7" s="10">
         <v>16308</v>
       </c>
@@ -1049,14 +1894,32 @@
       <c r="D7" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="3"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-    </row>
-    <row r="8" spans="2:11">
+      <c r="E7" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="K7" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="L7" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="M7" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13">
       <c r="B8" s="10">
         <v>16338</v>
       </c>
@@ -1066,14 +1929,32 @@
       <c r="D8" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="3"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-    </row>
-    <row r="9" spans="2:11">
+      <c r="E8" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I8" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J8" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="K8" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="L8" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="M8" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13">
       <c r="B9" s="10">
         <v>16339</v>
       </c>
@@ -1083,44 +1964,74 @@
       <c r="D9" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="3"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-    </row>
-    <row r="10" spans="2:11">
+      <c r="E9" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="K9" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="L9" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="M9" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13">
       <c r="B10" s="10">
         <v>16340</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="13"/>
+      <c r="D10" s="14" t="s">
+        <v>14</v>
+      </c>
       <c r="E10" s="3"/>
       <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
+      <c r="H10" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="I10" s="10"/>
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
-    </row>
-    <row r="11" spans="2:11">
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+    </row>
+    <row r="11" spans="2:13">
       <c r="B11" s="10">
         <v>16354</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="13"/>
+      <c r="D11" s="14" t="s">
+        <v>14</v>
+      </c>
       <c r="E11" s="3"/>
       <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
+      <c r="H11" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="I11" s="10"/>
       <c r="J11" s="10"/>
       <c r="K11" s="10"/>
-    </row>
-    <row r="12" spans="2:11">
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+    </row>
+    <row r="12" spans="2:13">
       <c r="B12" s="10">
         <v>16374</v>
       </c>
@@ -1130,14 +2041,32 @@
       <c r="D12" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="3"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-    </row>
-    <row r="13" spans="2:11">
+      <c r="E12" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J12" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="K12" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="L12" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="M12" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13">
       <c r="B13" s="10">
         <v>16401</v>
       </c>
@@ -1151,8 +2080,10 @@
       <c r="I13" s="10"/>
       <c r="J13" s="10"/>
       <c r="K13" s="10"/>
-    </row>
-    <row r="14" spans="2:11">
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+    </row>
+    <row r="14" spans="2:13">
       <c r="B14" s="10">
         <v>16402</v>
       </c>
@@ -1166,8 +2097,10 @@
       <c r="I14" s="10"/>
       <c r="J14" s="10"/>
       <c r="K14" s="10"/>
-    </row>
-    <row r="15" spans="2:11">
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+    </row>
+    <row r="15" spans="2:13">
       <c r="B15" s="10">
         <v>16403</v>
       </c>
@@ -1181,38 +2114,52 @@
       <c r="I15" s="10"/>
       <c r="J15" s="10"/>
       <c r="K15" s="10"/>
-    </row>
-    <row r="16" spans="2:11">
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+    </row>
+    <row r="16" spans="2:13">
       <c r="B16" s="10">
         <v>16404</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="13"/>
+      <c r="D16" s="9" t="s">
+        <v>20</v>
+      </c>
       <c r="E16" s="3"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
+      <c r="H16" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="I16" s="10"/>
       <c r="J16" s="10"/>
       <c r="K16" s="10"/>
-    </row>
-    <row r="17" spans="2:11" ht="30">
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
+    </row>
+    <row r="17" spans="2:13" ht="30">
       <c r="B17" s="10">
         <v>16405</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="13"/>
+      <c r="D17" s="9" t="s">
+        <v>20</v>
+      </c>
       <c r="E17" s="3"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
+      <c r="H17" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="I17" s="10"/>
       <c r="J17" s="10"/>
       <c r="K17" s="10"/>
-    </row>
-    <row r="18" spans="2:11" ht="30">
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
+    </row>
+    <row r="18" spans="2:13" ht="30">
       <c r="B18" s="10">
         <v>16411</v>
       </c>
@@ -1222,14 +2169,32 @@
       <c r="D18" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E18" s="3"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
-    </row>
-    <row r="19" spans="2:11">
+      <c r="E18" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="H18" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I18" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J18" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="K18" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="L18" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="M18" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13">
       <c r="B19" s="10">
         <v>16562</v>
       </c>
@@ -1239,14 +2204,32 @@
       <c r="D19" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E19" s="3"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
-      <c r="K19" s="10"/>
-    </row>
-    <row r="20" spans="2:11">
+      <c r="E19" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="H19" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I19" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J19" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="K19" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="L19" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="M19" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13">
       <c r="B20" s="10">
         <v>16563</v>
       </c>
@@ -1256,47 +2239,286 @@
       <c r="D20" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E20" s="3"/>
+      <c r="E20" s="8" t="s">
+        <v>14</v>
+      </c>
       <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
+      <c r="H20" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="I20" s="10"/>
       <c r="J20" s="10"/>
       <c r="K20" s="10"/>
-    </row>
-    <row r="21" spans="2:11">
+      <c r="L20" s="10"/>
+      <c r="M20" s="10"/>
+    </row>
+    <row r="21" spans="2:13">
       <c r="B21" s="10">
         <v>16564</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D21" s="12"/>
+      <c r="D21" s="9" t="s">
+        <v>20</v>
+      </c>
       <c r="E21" s="3"/>
       <c r="G21" s="10"/>
-      <c r="H21" s="10"/>
+      <c r="H21" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="I21" s="10"/>
       <c r="J21" s="10"/>
       <c r="K21" s="10"/>
-    </row>
-    <row r="22" spans="2:11">
+      <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
+    </row>
+    <row r="22" spans="2:13">
       <c r="B22" s="10">
         <v>16565</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D22" s="12"/>
+      <c r="D22" s="8" t="s">
+        <v>14</v>
+      </c>
       <c r="E22" s="3"/>
       <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
+      <c r="H22" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="I22" s="10"/>
       <c r="J22" s="10"/>
       <c r="K22" s="10"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="10"/>
+    </row>
+    <row r="23" spans="2:13" ht="30">
+      <c r="B23" s="10">
+        <v>16655</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" s="3"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="10"/>
+    </row>
+    <row r="24" spans="2:13" ht="45">
+      <c r="B24" s="10">
+        <v>16885</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24" s="3"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="10"/>
+    </row>
+    <row r="25" spans="2:13">
+      <c r="B25" s="10">
+        <v>16886</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" s="12"/>
+      <c r="E25" s="3"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="10"/>
+      <c r="M25" s="10"/>
+    </row>
+    <row r="26" spans="2:13" ht="60">
+      <c r="B26" s="10">
+        <v>17048</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E26" s="3"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I26" s="10"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="10"/>
+      <c r="M26" s="10"/>
+    </row>
+    <row r="27" spans="2:13" ht="30">
+      <c r="B27" s="10">
+        <v>17064</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E27" s="3"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="10"/>
+      <c r="M27" s="10"/>
+    </row>
+    <row r="28" spans="2:13" ht="30">
+      <c r="B28" s="10">
+        <v>17066</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E28" s="3"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I28" s="10"/>
+      <c r="J28" s="10"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="10"/>
+      <c r="M28" s="10"/>
+    </row>
+    <row r="29" spans="2:13">
+      <c r="B29" s="10">
+        <v>17067</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E29" s="3"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I29" s="10"/>
+      <c r="J29" s="10"/>
+      <c r="K29" s="10"/>
+      <c r="L29" s="10"/>
+      <c r="M29" s="10"/>
+    </row>
+    <row r="30" spans="2:13">
+      <c r="B30" s="10">
+        <v>17305</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D30" s="12"/>
+      <c r="E30" s="3"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I30" s="10"/>
+      <c r="J30" s="10"/>
+      <c r="K30" s="10"/>
+      <c r="L30" s="10"/>
+      <c r="M30" s="10"/>
+    </row>
+    <row r="31" spans="2:13" ht="30">
+      <c r="B31" s="10">
+        <v>17337</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E31" s="3"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I31" s="10"/>
+      <c r="J31" s="10"/>
+      <c r="K31" s="10"/>
+      <c r="L31" s="10"/>
+      <c r="M31" s="10"/>
+    </row>
+    <row r="32" spans="2:13">
+      <c r="B32" s="10"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="3"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="10"/>
+      <c r="J32" s="10"/>
+      <c r="K32" s="10"/>
+      <c r="L32" s="10"/>
+      <c r="M32" s="10"/>
+    </row>
+    <row r="33" spans="2:13">
+      <c r="B33" s="10"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="3"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="10"/>
+      <c r="J33" s="10"/>
+      <c r="K33" s="10"/>
+      <c r="L33" s="10"/>
+      <c r="M33" s="10"/>
+    </row>
+    <row r="34" spans="2:13">
+      <c r="B34" s="10"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="3"/>
+      <c r="G34" s="10"/>
+      <c r="H34" s="10"/>
+      <c r="I34" s="10"/>
+      <c r="J34" s="10"/>
+      <c r="K34" s="10"/>
+      <c r="L34" s="10"/>
+      <c r="M34" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Finalized Batch3 issues to be voted
</commit_message>
<xml_diff>
--- a/docs/dds-psm-cxx-ftf-votes.xlsx
+++ b/docs/dds-psm-cxx-ftf-votes.xlsx
@@ -1370,7 +1370,7 @@
   <dimension ref="B2:M18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1769,7 +1769,7 @@
   <dimension ref="B2:M34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
ISSUE:17305 Updated support for X-Types
</commit_message>
<xml_diff>
--- a/docs/dds-psm-cxx-ftf-votes.xlsx
+++ b/docs/dds-psm-cxx-ftf-votes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22624"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="100" yWindow="20" windowWidth="24560" windowHeight="18340" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="2000" yWindow="300" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="batch1" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="46">
   <si>
     <t>Issue #</t>
   </si>
@@ -123,9 +123,6 @@
   </si>
   <si>
     <t>Abstain</t>
-  </si>
-  <si>
-    <t>yes</t>
   </si>
   <si>
     <t>The tdds namespace should be merged into the dds namespace</t>
@@ -168,7 +165,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -221,9 +218,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="9" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="12"/>
-      <color rgb="FF808080"/>
+      <color theme="9" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
@@ -287,7 +290,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="223">
+  <cellStyleXfs count="251">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -511,8 +514,36 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -548,14 +579,30 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="223">
+  <cellStyles count="251">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
@@ -667,6 +714,20 @@
     <cellStyle name="Lien hypertexte" xfId="217" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="219" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="221" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="223" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="225" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="227" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="229" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="231" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="233" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="235" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="237" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="239" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="241" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="243" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="245" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="247" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="249" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
@@ -778,6 +839,20 @@
     <cellStyle name="Lien hypertexte visité" xfId="218" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="220" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="222" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="224" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="226" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="228" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="230" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="232" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="234" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="236" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="238" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="240" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="242" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="244" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="246" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="248" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="250" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1369,8 +1444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:M18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1411,10 +1486,10 @@
         <v>5</v>
       </c>
       <c r="L2" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="M2" s="7" t="s">
         <v>43</v>
-      </c>
-      <c r="M2" s="7" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="3" spans="2:13">
@@ -1424,18 +1499,28 @@
       <c r="C3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="3"/>
-      <c r="G3" s="10"/>
+      <c r="D3" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="H3" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="I3" s="10"/>
+      <c r="I3" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
+      <c r="K3" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="M3" s="10"/>
     </row>
     <row r="4" spans="2:13">
@@ -1445,18 +1530,28 @@
       <c r="C4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="3"/>
-      <c r="G4" s="10"/>
+      <c r="D4" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="H4" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="I4" s="10"/>
+      <c r="I4" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
+      <c r="K4" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="M4" s="10"/>
     </row>
     <row r="5" spans="2:13">
@@ -1469,15 +1564,25 @@
       <c r="D5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="3"/>
-      <c r="G5" s="10"/>
+      <c r="E5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="H5" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="I5" s="10"/>
+      <c r="I5" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
+      <c r="K5" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="L5" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="M5" s="10"/>
     </row>
     <row r="6" spans="2:13">
@@ -1487,18 +1592,28 @@
       <c r="C6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="3"/>
-      <c r="G6" s="10"/>
+      <c r="D6" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="H6" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="I6" s="10"/>
+      <c r="I6" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
+      <c r="K6" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="L6" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="M6" s="10"/>
     </row>
     <row r="7" spans="2:13">
@@ -1508,18 +1623,28 @@
       <c r="C7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="3"/>
-      <c r="G7" s="10"/>
+      <c r="D7" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="H7" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="I7" s="10"/>
+      <c r="I7" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
+      <c r="K7" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="L7" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="M7" s="10"/>
     </row>
     <row r="8" spans="2:13">
@@ -1529,18 +1654,28 @@
       <c r="C8" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="3"/>
-      <c r="G8" s="10"/>
+      <c r="D8" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="H8" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="I8" s="10"/>
+      <c r="I8" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
+      <c r="K8" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="L8" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="M8" s="10"/>
     </row>
     <row r="9" spans="2:13" ht="30">
@@ -1550,18 +1685,28 @@
       <c r="C9" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="3"/>
-      <c r="G9" s="10"/>
+      <c r="D9" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="H9" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="I9" s="10"/>
+      <c r="I9" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
+      <c r="K9" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="L9" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="M9" s="10"/>
     </row>
     <row r="10" spans="2:13">
@@ -1574,15 +1719,25 @@
       <c r="D10" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="3"/>
-      <c r="G10" s="10"/>
+      <c r="E10" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="H10" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="I10" s="10"/>
+      <c r="I10" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
+      <c r="K10" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="L10" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="M10" s="10"/>
     </row>
     <row r="11" spans="2:13">
@@ -1595,15 +1750,23 @@
       <c r="D11" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="3"/>
-      <c r="G11" s="10"/>
+      <c r="E11" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="H11" s="10" t="s">
         <v>31</v>
       </c>
       <c r="I11" s="10"/>
       <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
+      <c r="K11" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="L11" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="M11" s="10"/>
     </row>
     <row r="12" spans="2:13" ht="30">
@@ -1611,20 +1774,30 @@
         <v>16655</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D12" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="3"/>
-      <c r="G12" s="10"/>
+      <c r="E12" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="H12" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="I12" s="10"/>
+      <c r="I12" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
+      <c r="K12" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="L12" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="M12" s="10"/>
     </row>
     <row r="13" spans="2:13" ht="45">
@@ -1632,20 +1805,28 @@
         <v>16885</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D13" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="3"/>
-      <c r="G13" s="10"/>
+      <c r="E13" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="H13" s="10" t="s">
         <v>31</v>
       </c>
       <c r="I13" s="10"/>
       <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
+      <c r="K13" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="L13" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="M13" s="10"/>
     </row>
     <row r="14" spans="2:13" ht="60">
@@ -1653,20 +1834,30 @@
         <v>17048</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D14" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="3"/>
-      <c r="G14" s="10"/>
+      <c r="E14" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="H14" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="I14" s="10"/>
+      <c r="I14" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
+      <c r="K14" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="L14" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="M14" s="10"/>
     </row>
     <row r="15" spans="2:13" ht="30">
@@ -1674,20 +1865,30 @@
         <v>17064</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="3"/>
-      <c r="G15" s="10"/>
+      <c r="E15" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="H15" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="I15" s="10"/>
+      <c r="I15" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
+      <c r="K15" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="L15" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="M15" s="10"/>
     </row>
     <row r="16" spans="2:13" ht="30">
@@ -1695,20 +1896,30 @@
         <v>17066</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E16" s="3"/>
-      <c r="G16" s="10"/>
+      <c r="E16" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="H16" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="I16" s="10"/>
+      <c r="I16" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="J16" s="10"/>
-      <c r="K16" s="10"/>
-      <c r="L16" s="10"/>
+      <c r="K16" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="L16" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="M16" s="10"/>
     </row>
     <row r="17" spans="2:13">
@@ -1716,20 +1927,30 @@
         <v>17067</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="3"/>
-      <c r="G17" s="10"/>
+      <c r="E17" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="H17" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="I17" s="10"/>
+      <c r="I17" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="J17" s="10"/>
-      <c r="K17" s="10"/>
-      <c r="L17" s="10"/>
+      <c r="K17" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="L17" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="M17" s="10"/>
     </row>
     <row r="18" spans="2:13" ht="30">
@@ -1737,20 +1958,30 @@
         <v>17337</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E18" s="3"/>
-      <c r="G18" s="10"/>
+      <c r="E18" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="H18" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="I18" s="10"/>
+      <c r="I18" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
-      <c r="L18" s="10"/>
+      <c r="K18" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="L18" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="M18" s="10"/>
     </row>
   </sheetData>
@@ -1768,8 +1999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:M34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView topLeftCell="B14" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1810,10 +2041,10 @@
         <v>5</v>
       </c>
       <c r="L2" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="M2" s="7" t="s">
         <v>43</v>
-      </c>
-      <c r="M2" s="7" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="3" spans="2:13">
@@ -1823,18 +2054,28 @@
       <c r="C3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="3"/>
-      <c r="G3" s="10"/>
+      <c r="D3" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="H3" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="I3" s="10"/>
+      <c r="I3" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
+      <c r="K3" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="M3" s="10"/>
     </row>
     <row r="4" spans="2:13">
@@ -1844,28 +2085,38 @@
       <c r="C4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="3"/>
-      <c r="G4" s="10"/>
+      <c r="D4" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="H4" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="I4" s="10"/>
+      <c r="I4" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
+      <c r="K4" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="M4" s="10"/>
     </row>
     <row r="5" spans="2:13">
-      <c r="B5" s="10">
+      <c r="B5" s="14">
         <v>16261</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="12"/>
+      <c r="D5" s="20"/>
       <c r="E5" s="3"/>
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
@@ -1885,15 +2136,25 @@
       <c r="D6" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="3"/>
-      <c r="G6" s="10"/>
+      <c r="E6" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="H6" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="I6" s="10"/>
+      <c r="I6" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
+      <c r="K6" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="L6" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="M6" s="10"/>
     </row>
     <row r="7" spans="2:13">
@@ -1925,10 +2186,10 @@
         <v>31</v>
       </c>
       <c r="L7" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M7" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="2:13">
@@ -1960,10 +2221,10 @@
         <v>31</v>
       </c>
       <c r="L8" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M8" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="2:13">
@@ -1995,10 +2256,10 @@
         <v>31</v>
       </c>
       <c r="L9" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M9" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="2:13">
@@ -2008,18 +2269,28 @@
       <c r="C10" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="3"/>
-      <c r="G10" s="10"/>
+      <c r="D10" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="H10" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="I10" s="10"/>
+      <c r="I10" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
+      <c r="K10" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="L10" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="M10" s="10"/>
     </row>
     <row r="11" spans="2:13">
@@ -2029,18 +2300,28 @@
       <c r="C11" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" s="3"/>
-      <c r="G11" s="10"/>
+      <c r="D11" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="H11" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="I11" s="10"/>
+      <c r="I11" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
+      <c r="K11" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="L11" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="M11" s="10"/>
     </row>
     <row r="12" spans="2:13">
@@ -2072,21 +2353,21 @@
         <v>31</v>
       </c>
       <c r="L12" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M12" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="2:13">
-      <c r="B13" s="10">
+      <c r="B13" s="14">
         <v>16401</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="13"/>
-      <c r="E13" s="3"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="18"/>
       <c r="G13" s="10"/>
       <c r="H13" s="10"/>
       <c r="I13" s="10"/>
@@ -2096,14 +2377,14 @@
       <c r="M13" s="10"/>
     </row>
     <row r="14" spans="2:13">
-      <c r="B14" s="10">
+      <c r="B14" s="14">
         <v>16402</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="13"/>
-      <c r="E14" s="3"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="18"/>
       <c r="G14" s="10"/>
       <c r="H14" s="10"/>
       <c r="I14" s="10"/>
@@ -2113,14 +2394,14 @@
       <c r="M14" s="10"/>
     </row>
     <row r="15" spans="2:13">
-      <c r="B15" s="10">
+      <c r="B15" s="14">
         <v>16403</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="13"/>
-      <c r="E15" s="3"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="18"/>
       <c r="G15" s="10"/>
       <c r="H15" s="10"/>
       <c r="I15" s="10"/>
@@ -2136,18 +2417,28 @@
       <c r="C16" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E16" s="3"/>
-      <c r="G16" s="10"/>
+      <c r="D16" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="H16" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="I16" s="10"/>
+      <c r="I16" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="J16" s="10"/>
-      <c r="K16" s="10"/>
-      <c r="L16" s="10"/>
+      <c r="K16" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="L16" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="M16" s="10"/>
     </row>
     <row r="17" spans="2:13" ht="30">
@@ -2157,18 +2448,28 @@
       <c r="C17" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E17" s="3"/>
-      <c r="G17" s="10"/>
+      <c r="D17" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="H17" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="I17" s="10"/>
+      <c r="I17" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="J17" s="10"/>
-      <c r="K17" s="10"/>
-      <c r="L17" s="10"/>
+      <c r="K17" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="L17" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="M17" s="10"/>
     </row>
     <row r="18" spans="2:13" ht="30">
@@ -2197,13 +2498,13 @@
         <v>31</v>
       </c>
       <c r="K18" s="10" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="L18" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M18" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="2:13">
@@ -2232,13 +2533,13 @@
         <v>31</v>
       </c>
       <c r="K19" s="10" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="L19" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M19" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="2:13">
@@ -2254,14 +2555,22 @@
       <c r="E20" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="G20" s="10"/>
+      <c r="G20" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="H20" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="I20" s="10"/>
+      <c r="I20" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="J20" s="10"/>
-      <c r="K20" s="10"/>
-      <c r="L20" s="10"/>
+      <c r="K20" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="L20" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="M20" s="10"/>
     </row>
     <row r="21" spans="2:13">
@@ -2274,15 +2583,25 @@
       <c r="D21" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E21" s="3"/>
-      <c r="G21" s="10"/>
+      <c r="E21" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="H21" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="I21" s="10"/>
+      <c r="I21" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="J21" s="10"/>
-      <c r="K21" s="10"/>
-      <c r="L21" s="10"/>
+      <c r="K21" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="L21" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="M21" s="10"/>
     </row>
     <row r="22" spans="2:13">
@@ -2295,15 +2614,25 @@
       <c r="D22" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E22" s="3"/>
-      <c r="G22" s="10"/>
+      <c r="E22" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="H22" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="I22" s="10"/>
+      <c r="I22" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="J22" s="10"/>
-      <c r="K22" s="10"/>
-      <c r="L22" s="10"/>
+      <c r="K22" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="L22" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="M22" s="10"/>
     </row>
     <row r="23" spans="2:13" ht="30">
@@ -2311,20 +2640,30 @@
         <v>16655</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D23" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E23" s="3"/>
-      <c r="G23" s="10"/>
+      <c r="E23" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="H23" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="I23" s="10"/>
+      <c r="I23" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="J23" s="10"/>
-      <c r="K23" s="10"/>
-      <c r="L23" s="10"/>
+      <c r="K23" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="L23" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="M23" s="10"/>
     </row>
     <row r="24" spans="2:13" ht="45">
@@ -2332,30 +2671,40 @@
         <v>16885</v>
       </c>
       <c r="C24" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G24" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="H24" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I24" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="L24" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="M24" s="10"/>
+    </row>
+    <row r="25" spans="2:13">
+      <c r="B25" s="14">
+        <v>16886</v>
+      </c>
+      <c r="C25" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D24" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E24" s="3"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="I24" s="10"/>
-      <c r="J24" s="10"/>
-      <c r="K24" s="10"/>
-      <c r="L24" s="10"/>
-      <c r="M24" s="10"/>
-    </row>
-    <row r="25" spans="2:13">
-      <c r="B25" s="10">
-        <v>16886</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D25" s="12"/>
+      <c r="D25" s="16"/>
       <c r="E25" s="3"/>
       <c r="G25" s="10"/>
       <c r="H25" s="10"/>
@@ -2370,20 +2719,30 @@
         <v>17048</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D26" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E26" s="3"/>
-      <c r="G26" s="10"/>
+      <c r="E26" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G26" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="H26" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="I26" s="10"/>
+      <c r="I26" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="J26" s="10"/>
-      <c r="K26" s="10"/>
-      <c r="L26" s="10"/>
+      <c r="K26" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="L26" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="M26" s="10"/>
     </row>
     <row r="27" spans="2:13" ht="30">
@@ -2391,20 +2750,30 @@
         <v>17064</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D27" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E27" s="3"/>
-      <c r="G27" s="10"/>
+      <c r="E27" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G27" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="H27" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="I27" s="10"/>
+      <c r="I27" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="J27" s="10"/>
-      <c r="K27" s="10"/>
-      <c r="L27" s="10"/>
+      <c r="K27" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="L27" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="M27" s="10"/>
     </row>
     <row r="28" spans="2:13" ht="30">
@@ -2412,20 +2781,30 @@
         <v>17066</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D28" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E28" s="3"/>
-      <c r="G28" s="10"/>
+      <c r="E28" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G28" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="H28" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="I28" s="10"/>
+      <c r="I28" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="J28" s="10"/>
-      <c r="K28" s="10"/>
-      <c r="L28" s="10"/>
+      <c r="K28" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="L28" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="M28" s="10"/>
     </row>
     <row r="29" spans="2:13">
@@ -2433,39 +2812,57 @@
         <v>17067</v>
       </c>
       <c r="C29" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E29" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G29" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="H29" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I29" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J29" s="10"/>
+      <c r="K29" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="L29" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="M29" s="10"/>
+    </row>
+    <row r="30" spans="2:13">
+      <c r="B30" s="14">
+        <v>17305</v>
+      </c>
+      <c r="C30" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="D29" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E29" s="3"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="I29" s="10"/>
-      <c r="J29" s="10"/>
-      <c r="K29" s="10"/>
-      <c r="L29" s="10"/>
-      <c r="M29" s="10"/>
-    </row>
-    <row r="30" spans="2:13">
-      <c r="B30" s="10">
-        <v>17305</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D30" s="12"/>
-      <c r="E30" s="3"/>
-      <c r="G30" s="10"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="18"/>
+      <c r="G30" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="H30" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="I30" s="10"/>
+      <c r="I30" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="J30" s="10"/>
-      <c r="K30" s="10"/>
-      <c r="L30" s="10"/>
+      <c r="K30" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="L30" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="M30" s="10"/>
     </row>
     <row r="31" spans="2:13" ht="30">
@@ -2473,20 +2870,30 @@
         <v>17337</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D31" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E31" s="3"/>
-      <c r="G31" s="10"/>
+      <c r="E31" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G31" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="H31" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="I31" s="10"/>
+      <c r="I31" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="J31" s="10"/>
-      <c r="K31" s="10"/>
-      <c r="L31" s="10"/>
+      <c r="K31" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="L31" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="M31" s="10"/>
     </row>
     <row r="32" spans="2:13">

</xml_diff>

<commit_message>
Fixed Indendation. Now 2 spaces are used consistently across the code
</commit_message>
<xml_diff>
--- a/docs/dds-psm-cxx-ftf-votes.xlsx
+++ b/docs/dds-psm-cxx-ftf-votes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22624"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2000" yWindow="300" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="2000" yWindow="300" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="batch1" sheetId="2" r:id="rId1"/>
@@ -1444,7 +1444,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:M18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -1999,8 +1999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:M34"/>
   <sheetViews>
-    <sheetView topLeftCell="B14" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="B20" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>